<commit_message>
Aggiornamento casi di test
Come da mail aggiorniamo i file per l'accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/SCC/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/SCC/1.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\S1#060000000000XX\INSIEL\SCC\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B31C3E9-775F-466A-BB6E-8DF6FFEE155F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84589070-FEAC-46DC-8FED-521CD572871F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26595" windowHeight="15750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="879">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4658,48 +4658,6 @@
     <t>subject_application_version:1.0.0</t>
   </si>
   <si>
-    <t>2024-03-05T08:14:00Z</t>
-  </si>
-  <si>
-    <t>2024-03-05T08:15:00Z</t>
-  </si>
-  <si>
-    <t>2024-03-05T08:16:00Z</t>
-  </si>
-  <si>
-    <t>2024-03-05T08:17:00Z</t>
-  </si>
-  <si>
-    <t>b283e6d5e1eda740</t>
-  </si>
-  <si>
-    <t>a385b9c734f79ae7</t>
-  </si>
-  <si>
-    <t>2bb195530085b6e8</t>
-  </si>
-  <si>
-    <t>2ad82a2b65b14f56</t>
-  </si>
-  <si>
-    <t>8e3cfbd9cbb6b8cd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.b3ecbb15fe2799d1b3991573275e1c7001eef1c6a3cdd48ee2bc8fcf3059f936.a46063bbb0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.b967f3228691a54408afcb6884e5ff7e73dbdbcb33b08744fb6d2182dec44ccd.d008220d0c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.96ea4311f3946ad2fed588693a4db7284e094d5c7a4df0eb09f1243e6afab8fe.babe9218b8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.145941d8c39205a282dc7c1a70b1ff994ee173af5840b206cc7637da72ad0ac6.ec9d01b3e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.a81553b1dc890bbd36fa4a435ebe7fc6c2e8065d56efcd57fa594aa833128fb9.903e5da2df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Viene scritto un log con i dettagli d'errore, se l'errore persiste o ci sono lamentele dal utente si procede con le solite verifiche di raggiungibilità con eventuale email al fornitore del servizio.</t>
   </si>
   <si>
@@ -4740,6 +4698,39 @@
   </si>
   <si>
     <t>Caso non applicabile nel software di cartella, il valore non può essere variato da "S"</t>
+  </si>
+  <si>
+    <t>2024-03-08T11:41:00Z</t>
+  </si>
+  <si>
+    <t>88132e1095a31af3</t>
+  </si>
+  <si>
+    <t>9d8e1cf3073e79f1</t>
+  </si>
+  <si>
+    <t>2ca4f009fd3c6447</t>
+  </si>
+  <si>
+    <t>e1ff40364353babc</t>
+  </si>
+  <si>
+    <t>66f1061528cad8af</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.7373869581ea57d9eed937dd9e572ffa5d46554df4727e02d2ee5230c37538ce.24c0aa679b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.9e28feb8ec6ee94534fb548d47d14c7c2f191d4cdb6f3a8168897898fe4aa2f2.47914af06b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.c1084071dfcf9886b03149b8ad4b229618f44f799eb20d6ffe5583949536e100.ea3878989f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.5346cf38f629aa65336d19d03d1401ec5602918d9f4abe021e11da0d71103ee1.7f4b6e338b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.c5762e20912fd7d0f0327214a500162d32541a50d21bafb961d3616c3cd9f605.9628c84c03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -5085,7 +5076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5201,6 +5192,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7667,7 +7661,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K197" sqref="K197"/>
+      <selection pane="bottomRight" activeCell="I180" sqref="I180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8866,7 +8860,7 @@
         <v>847</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>869</v>
+        <v>855</v>
       </c>
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
@@ -9142,7 +9136,7 @@
         <v>847</v>
       </c>
       <c r="K45" s="25" t="s">
-        <v>869</v>
+        <v>855</v>
       </c>
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
@@ -9435,7 +9429,7 @@
         <v>847</v>
       </c>
       <c r="P53" s="25" t="s">
-        <v>868</v>
+        <v>854</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">
@@ -13655,16 +13649,16 @@
         <v>383</v>
       </c>
       <c r="F177" s="23">
-        <v>45356</v>
+        <v>45359</v>
       </c>
       <c r="G177" s="24" t="s">
-        <v>855</v>
+        <v>868</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>861</v>
+        <v>870</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>866</v>
+        <v>875</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -13699,16 +13693,16 @@
         <v>385</v>
       </c>
       <c r="F178" s="23">
-        <v>45356</v>
+        <v>45359</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>856</v>
+        <v>868</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>860</v>
+        <v>871</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>865</v>
+        <v>876</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -13743,16 +13737,16 @@
         <v>387</v>
       </c>
       <c r="F179" s="23">
-        <v>45356</v>
+        <v>45359</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>856</v>
+        <v>868</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>859</v>
+        <v>872</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>864</v>
+        <v>877</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -13787,16 +13781,16 @@
         <v>389</v>
       </c>
       <c r="F180" s="23">
-        <v>45356</v>
+        <v>45359</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>857</v>
+        <v>868</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>858</v>
-      </c>
-      <c r="I180" s="24" t="s">
-        <v>863</v>
+        <v>873</v>
+      </c>
+      <c r="I180" s="48" t="s">
+        <v>878</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -13838,7 +13832,7 @@
         <v>847</v>
       </c>
       <c r="K181" s="25" t="s">
-        <v>870</v>
+        <v>856</v>
       </c>
       <c r="L181" s="25"/>
       <c r="M181" s="25"/>
@@ -13876,7 +13870,7 @@
         <v>847</v>
       </c>
       <c r="K182" s="25" t="s">
-        <v>871</v>
+        <v>857</v>
       </c>
       <c r="L182" s="25"/>
       <c r="M182" s="25"/>
@@ -13914,7 +13908,7 @@
         <v>847</v>
       </c>
       <c r="K183" s="25" t="s">
-        <v>872</v>
+        <v>858</v>
       </c>
       <c r="L183" s="25"/>
       <c r="M183" s="25"/>
@@ -13952,7 +13946,7 @@
         <v>847</v>
       </c>
       <c r="K184" s="25" t="s">
-        <v>873</v>
+        <v>859</v>
       </c>
       <c r="L184" s="25"/>
       <c r="M184" s="25"/>
@@ -13990,7 +13984,7 @@
         <v>847</v>
       </c>
       <c r="K185" s="35" t="s">
-        <v>873</v>
+        <v>859</v>
       </c>
       <c r="L185" s="25"/>
       <c r="M185" s="25"/>
@@ -14028,7 +14022,7 @@
         <v>847</v>
       </c>
       <c r="K186" s="25" t="s">
-        <v>873</v>
+        <v>859</v>
       </c>
       <c r="L186" s="25"/>
       <c r="M186" s="25"/>
@@ -14066,7 +14060,7 @@
         <v>847</v>
       </c>
       <c r="K187" s="25" t="s">
-        <v>874</v>
+        <v>860</v>
       </c>
       <c r="L187" s="25"/>
       <c r="M187" s="25"/>
@@ -14104,7 +14098,7 @@
         <v>847</v>
       </c>
       <c r="K188" s="25" t="s">
-        <v>875</v>
+        <v>861</v>
       </c>
       <c r="L188" s="25"/>
       <c r="M188" s="25"/>
@@ -14142,7 +14136,7 @@
         <v>847</v>
       </c>
       <c r="K189" s="25" t="s">
-        <v>876</v>
+        <v>862</v>
       </c>
       <c r="L189" s="25"/>
       <c r="M189" s="25"/>
@@ -14180,7 +14174,7 @@
         <v>847</v>
       </c>
       <c r="K190" s="25" t="s">
-        <v>877</v>
+        <v>863</v>
       </c>
       <c r="L190" s="25"/>
       <c r="M190" s="25"/>
@@ -14218,7 +14212,7 @@
         <v>847</v>
       </c>
       <c r="K191" s="25" t="s">
-        <v>878</v>
+        <v>864</v>
       </c>
       <c r="L191" s="25"/>
       <c r="M191" s="25"/>
@@ -14256,7 +14250,7 @@
         <v>847</v>
       </c>
       <c r="K192" s="25" t="s">
-        <v>879</v>
+        <v>865</v>
       </c>
       <c r="L192" s="25"/>
       <c r="M192" s="25"/>
@@ -14294,7 +14288,7 @@
         <v>847</v>
       </c>
       <c r="K193" s="25" t="s">
-        <v>879</v>
+        <v>865</v>
       </c>
       <c r="L193" s="25"/>
       <c r="M193" s="25"/>
@@ -14332,7 +14326,7 @@
         <v>847</v>
       </c>
       <c r="K194" s="25" t="s">
-        <v>879</v>
+        <v>865</v>
       </c>
       <c r="L194" s="25"/>
       <c r="M194" s="25"/>
@@ -14370,7 +14364,7 @@
         <v>847</v>
       </c>
       <c r="K195" s="25" t="s">
-        <v>879</v>
+        <v>865</v>
       </c>
       <c r="L195" s="25"/>
       <c r="M195" s="25"/>
@@ -14408,7 +14402,7 @@
         <v>847</v>
       </c>
       <c r="K196" s="25" t="s">
-        <v>880</v>
+        <v>866</v>
       </c>
       <c r="L196" s="25"/>
       <c r="M196" s="25"/>
@@ -14446,7 +14440,7 @@
         <v>847</v>
       </c>
       <c r="K197" s="25" t="s">
-        <v>881</v>
+        <v>867</v>
       </c>
       <c r="L197" s="25"/>
       <c r="M197" s="25"/>
@@ -20733,16 +20727,16 @@
         <v>791</v>
       </c>
       <c r="F382" s="23">
-        <v>45356</v>
+        <v>45359</v>
       </c>
       <c r="G382" s="24" t="s">
-        <v>854</v>
+        <v>868</v>
       </c>
       <c r="H382" s="24" t="s">
-        <v>862</v>
+        <v>869</v>
       </c>
       <c r="I382" s="24" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
       <c r="J382" s="25" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
Aggiornamento dati come richiesto da email
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/SCC/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/SCC/1.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\S1#060000000000XX\INSIEL\SCC\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84589070-FEAC-46DC-8FED-521CD572871F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0F97DA-31BF-4E5D-893F-29575E279C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="881">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4700,37 +4700,43 @@
     <t>Caso non applicabile nel software di cartella, il valore non può essere variato da "S"</t>
   </si>
   <si>
-    <t>2024-03-08T11:41:00Z</t>
-  </si>
-  <si>
-    <t>88132e1095a31af3</t>
-  </si>
-  <si>
-    <t>9d8e1cf3073e79f1</t>
-  </si>
-  <si>
-    <t>2ca4f009fd3c6447</t>
-  </si>
-  <si>
-    <t>e1ff40364353babc</t>
-  </si>
-  <si>
-    <t>66f1061528cad8af</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.7373869581ea57d9eed937dd9e572ffa5d46554df4727e02d2ee5230c37538ce.24c0aa679b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.9e28feb8ec6ee94534fb548d47d14c7c2f191d4cdb6f3a8168897898fe4aa2f2.47914af06b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.c1084071dfcf9886b03149b8ad4b229618f44f799eb20d6ffe5583949536e100.ea3878989f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.5346cf38f629aa65336d19d03d1401ec5602918d9f4abe021e11da0d71103ee1.7f4b6e338b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.c5762e20912fd7d0f0327214a500162d32541a50d21bafb961d3616c3cd9f605.9628c84c03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-03-15T09:13:00Z</t>
+  </si>
+  <si>
+    <t>2024-03-15T09:14:00Z</t>
+  </si>
+  <si>
+    <t>fdf5b0152ee67d6f</t>
+  </si>
+  <si>
+    <t>f084f40797c9d160</t>
+  </si>
+  <si>
+    <t>752ff85d5c30a56f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.040d0f3bbb1f7feee81d8961a037dde1fdcdb75e684e8caaac794b4fc43d58ca.85eae7cdb9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.9e51807d9570dd70baeb5168825388a389dd6a681b272851346886cd57e7bb45.ed87d38687^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.f92fc1a0cd695dd20ee8cad558fec86fd3d4236387c809eb78d761791820f475.abf82ef705^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-18T08:23:00Z</t>
+  </si>
+  <si>
+    <t>513a5ea4361d79cd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.e2d1ee7bc769479ee1b3918fa3bf84304e8e6dce1ff516cc787b6b258e96c30d.1cc7bdbf74^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ded75e74088e93e2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.10c8f8ad95c8db6cab689d44b0c6038c77bd8a3b347b0d7668df5db05018b0ca.3482a66bec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -5171,6 +5177,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5192,9 +5201,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7658,10 +7664,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I180" sqref="I180"/>
+      <selection pane="bottomRight" activeCell="I181" sqref="I181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7702,14 +7708,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>851</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7727,14 +7733,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="48" t="s">
         <v>849</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="40"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7752,12 +7758,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="47" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="48" t="s">
         <v>850</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7776,12 +7782,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48" t="s">
         <v>853</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="40"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7799,8 +7805,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -13649,16 +13655,16 @@
         <v>383</v>
       </c>
       <c r="F177" s="23">
-        <v>45359</v>
+        <v>45366</v>
       </c>
       <c r="G177" s="24" t="s">
         <v>868</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -13693,16 +13699,16 @@
         <v>385</v>
       </c>
       <c r="F178" s="23">
-        <v>45359</v>
+        <v>45366</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -13737,16 +13743,16 @@
         <v>387</v>
       </c>
       <c r="F179" s="23">
-        <v>45359</v>
+        <v>45369</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -13781,16 +13787,16 @@
         <v>389</v>
       </c>
       <c r="F180" s="23">
-        <v>45359</v>
-      </c>
-      <c r="G180" s="24" t="s">
-        <v>868</v>
+        <v>45369</v>
+      </c>
+      <c r="G180" s="36" t="s">
+        <v>876</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>873</v>
-      </c>
-      <c r="I180" s="48" t="s">
-        <v>878</v>
+        <v>879</v>
+      </c>
+      <c r="I180" s="36" t="s">
+        <v>880</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -20727,16 +20733,16 @@
         <v>791</v>
       </c>
       <c r="F382" s="23">
-        <v>45359</v>
+        <v>45366</v>
       </c>
       <c r="G382" s="24" t="s">
         <v>868</v>
       </c>
       <c r="H382" s="24" t="s">
-        <v>869</v>
-      </c>
-      <c r="I382" s="24" t="s">
-        <v>874</v>
+        <v>870</v>
+      </c>
+      <c r="I382" s="36" t="s">
+        <v>875</v>
       </c>
       <c r="J382" s="25" t="s">
         <v>138</v>

</xml_diff>